<commit_message>
Updates phyloseq graphs for 12S and 16S; Updates 12S reference database
</commit_message>
<xml_diff>
--- a/DADA2/WADE003-arcticpred-12SP2-taxa2.xlsx
+++ b/DADA2/WADE003-arcticpred-12SP2-taxa2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/DADA2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="11_2716FDC58F79A8D366075C52F37BD2723ACB889C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0881A93-8459-4CBB-B4D5-27F0155683F5}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="11_2716FDC58F79A8D366075C52F37BD2723ACB889C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{283D44C1-F265-40DC-A732-B1312FA8F5A8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="319">
   <si>
     <t>rownames</t>
   </si>
@@ -947,9 +947,6 @@
   </si>
   <si>
     <t>Brachyopsis segaliensis; 6/28/25</t>
-  </si>
-  <si>
-    <t>no matcg</t>
   </si>
   <si>
     <t>Oncorhynchus gorbuscha; 6/28/25</t>
@@ -1004,12 +1001,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1022,6 +1020,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1032,8 +1035,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1041,9 +1045,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1349,7 +1354,7 @@
   <dimension ref="A1:I226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="I227" sqref="I227"/>
+      <selection activeCell="H225" sqref="H225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1362,7 @@
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
@@ -2293,29 +2298,29 @@
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="3" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2368,29 +2373,29 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="3" t="s">
         <v>300</v>
       </c>
     </row>
@@ -2734,26 +2739,26 @@
         <v>294</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="B59" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="3" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3145,23 +3150,23 @@
         <v>294</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B77" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="B77" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" s="3" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3271,29 +3276,29 @@
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="B83" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83" s="3" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3624,29 +3629,29 @@
         <v>294</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B99" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" t="s">
-        <v>10</v>
-      </c>
-      <c r="D99" t="s">
-        <v>12</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="B99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" s="3" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3794,17 +3799,17 @@
         <v>294</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B106" t="s">
-        <v>9</v>
-      </c>
-      <c r="C106" t="s">
-        <v>10</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="B106" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" s="3" t="s">
         <v>12</v>
       </c>
       <c r="I106" s="3" t="s">
@@ -4181,26 +4186,26 @@
         <v>294</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="124" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B124" t="s">
-        <v>9</v>
-      </c>
-      <c r="C124" t="s">
-        <v>10</v>
-      </c>
-      <c r="D124" t="s">
-        <v>12</v>
-      </c>
-      <c r="E124" t="s">
+      <c r="B124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F124" t="s">
+      <c r="F124" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I124" t="s">
+      <c r="I124" s="3" t="s">
         <v>308</v>
       </c>
     </row>
@@ -4247,29 +4252,29 @@
         <v>294</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="127" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B127" t="s">
-        <v>9</v>
-      </c>
-      <c r="C127" t="s">
-        <v>10</v>
-      </c>
-      <c r="D127" t="s">
-        <v>12</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="B127" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F127" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G127" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I127" t="s">
+      <c r="I127" s="3" t="s">
         <v>298</v>
       </c>
     </row>
@@ -4284,7 +4289,7 @@
         <v>10</v>
       </c>
       <c r="I128" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4599,30 +4604,30 @@
         <v>294</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="144" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B144" t="s">
-        <v>9</v>
-      </c>
-      <c r="C144" t="s">
-        <v>10</v>
-      </c>
-      <c r="D144" t="s">
-        <v>12</v>
-      </c>
-      <c r="E144" t="s">
+      <c r="B144" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E144" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F144" t="s">
+      <c r="F144" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G144" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I144" t="s">
-        <v>310</v>
+      <c r="I144" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -4777,24 +4782,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="152" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B152" t="s">
-        <v>9</v>
-      </c>
-      <c r="C152" t="s">
-        <v>10</v>
-      </c>
-      <c r="D152" t="s">
-        <v>12</v>
-      </c>
-      <c r="E152" t="s">
+      <c r="B152" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E152" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I152" t="s">
-        <v>311</v>
+      <c r="I152" s="3" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -4863,24 +4868,24 @@
         <v>294</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="156" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B156" t="s">
-        <v>9</v>
-      </c>
-      <c r="C156" t="s">
-        <v>10</v>
-      </c>
-      <c r="D156" t="s">
-        <v>12</v>
-      </c>
-      <c r="E156" t="s">
+      <c r="B156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E156" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I156" t="s">
-        <v>312</v>
+      <c r="I156" s="3" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -4963,18 +4968,18 @@
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="161" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B161" t="s">
-        <v>9</v>
-      </c>
-      <c r="C161" t="s">
-        <v>10</v>
-      </c>
-      <c r="I161" t="s">
-        <v>314</v>
+      <c r="B161" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5034,21 +5039,21 @@
         <v>294</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="165" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B165" t="s">
-        <v>9</v>
-      </c>
-      <c r="C165" t="s">
-        <v>10</v>
-      </c>
-      <c r="D165" t="s">
-        <v>12</v>
-      </c>
-      <c r="I165" t="s">
-        <v>313</v>
+      <c r="B165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5321,30 +5326,30 @@
         <v>294</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="181" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B181" t="s">
-        <v>9</v>
-      </c>
-      <c r="C181" t="s">
-        <v>10</v>
-      </c>
-      <c r="D181" t="s">
-        <v>12</v>
-      </c>
-      <c r="E181" t="s">
+      <c r="B181" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E181" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F181" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G181" t="s">
+      <c r="G181" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I181" t="s">
-        <v>315</v>
+      <c r="I181" s="3" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -5395,27 +5400,27 @@
         <v>294</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="185" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B185" t="s">
-        <v>9</v>
-      </c>
-      <c r="C185" t="s">
-        <v>10</v>
-      </c>
-      <c r="D185" t="s">
-        <v>12</v>
-      </c>
-      <c r="E185" t="s">
+      <c r="B185" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E185" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F185" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I185" t="s">
-        <v>316</v>
+      <c r="I185" s="3" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -5568,7 +5573,7 @@
         <v>10</v>
       </c>
       <c r="I194" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -5918,30 +5923,30 @@
         <v>294</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="214" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B214" t="s">
-        <v>9</v>
-      </c>
-      <c r="C214" t="s">
-        <v>10</v>
-      </c>
-      <c r="D214" t="s">
-        <v>12</v>
-      </c>
-      <c r="E214" t="s">
+      <c r="B214" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E214" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="F214" t="s">
+      <c r="F214" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G214" t="s">
+      <c r="G214" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="I214" t="s">
-        <v>318</v>
+      <c r="I214" s="3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -6087,30 +6092,30 @@
         <v>294</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="222" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B222" t="s">
-        <v>9</v>
-      </c>
-      <c r="C222" t="s">
-        <v>10</v>
-      </c>
-      <c r="D222" t="s">
-        <v>12</v>
-      </c>
-      <c r="E222" t="s">
+      <c r="B222" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E222" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F222" t="s">
+      <c r="F222" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G222" t="s">
+      <c r="G222" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="I222" t="s">
-        <v>319</v>
+      <c r="I222" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates phyloseq 12s and 16s with adjustments and a .csv output. adds species to 12s database; adds figures and DADA2 outputs
</commit_message>
<xml_diff>
--- a/DADA2/WADE003-arcticpred-12SP2-taxa2.xlsx
+++ b/DADA2/WADE003-arcticpred-12SP2-taxa2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1062,6 +1062,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1353,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="H225" sqref="H225"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>